<commit_message>
Added D2 Integration and Cal
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA03FLMB_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA03FLMB_00001.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7170" yWindow="8670" windowWidth="25950" windowHeight="10050" activeTab="1"/>
+    <workbookView xWindow="7170" yWindow="8670" windowWidth="25950" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -1374,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1454,9 @@
       <c r="F2" s="12">
         <v>0.10416666666666667</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7">
+        <v>42328</v>
+      </c>
       <c r="H2" s="3" t="s">
         <v>50</v>
       </c>
@@ -1498,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
corrected CTDMO reference designators to D1 cal sheet, add controllers to Integration sheet
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA03FLMB_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA03FLMB_00001.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7170" yWindow="8670" windowWidth="25950" windowHeight="10050"/>
+    <workbookView xWindow="7170" yWindow="8670" windowWidth="25950" windowHeight="10050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -208,40 +208,7 @@
     <t>GA03FLMB-RIM01-02-ADCPSL007</t>
   </si>
   <si>
-    <t>GA03FLMB-RIM01-02-CTDMOG043</t>
-  </si>
-  <si>
-    <t>GA03FLMB-RIM01-02-CTDMOG013</t>
-  </si>
-  <si>
-    <t>GA03FLMB-RIM01-02-CTDMOG044</t>
-  </si>
-  <si>
-    <t>GA03FLMB-RIM01-02-CTDMOG014</t>
-  </si>
-  <si>
-    <t>GA03FLMB-RIM01-02-CTDMOG047</t>
-  </si>
-  <si>
     <t>GA03FLMB-RIM01-02-CTDMOG065</t>
-  </si>
-  <si>
-    <t>GA03FLMB-RIM01-02-CTDMOG051</t>
-  </si>
-  <si>
-    <t>GA03FLMB-RIM01-02-CTDMOG050</t>
-  </si>
-  <si>
-    <t>GA03FLMB-RIM01-02-CTDMOG040</t>
-  </si>
-  <si>
-    <t>GA03FLMB-RIM01-02-CTDMOH095</t>
-  </si>
-  <si>
-    <t>GA03FLMB-RIM01-02-CTDMOH087</t>
-  </si>
-  <si>
-    <t>GA03FLMB-RIM01-02-CTDMOH088</t>
   </si>
   <si>
     <t>GA03FLMB-RIS01-04-PHSENF000</t>
@@ -374,6 +341,39 @@
   </si>
   <si>
     <t>OL000004</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOG060</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOG061</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOG062</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOG063</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOG064</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOG066</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOG067</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOG068</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOH069</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOH070</t>
+  </si>
+  <si>
+    <t>GA03FLMB-RIM01-02-CTDMOH071</t>
   </si>
 </sst>
 </file>
@@ -1374,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1399,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>0</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="2" spans="1:14" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>55</v>
@@ -1467,7 +1467,7 @@
         <v>5170</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="11">
@@ -1498,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1513,9 +1513,11 @@
     <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.7109375" style="2"/>
+    <col min="10" max="14" width="8.7109375" style="2"/>
+    <col min="15" max="15" width="9.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="23" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
@@ -1523,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>1</v>
@@ -1532,7 +1534,7 @@
         <v>41</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>2</v>
@@ -1552,7 +1554,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>47</v>
@@ -1561,7 +1563,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F2" s="13">
         <v>1219</v>
@@ -1584,7 +1586,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>47</v>
@@ -1593,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F3" s="13">
         <v>1219</v>
@@ -1613,7 +1615,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>47</v>
@@ -1622,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F4" s="13">
         <v>1219</v>
@@ -1639,7 +1641,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>47</v>
@@ -1648,7 +1650,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F5" s="13">
         <v>1219</v>
@@ -1665,7 +1667,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>47</v>
@@ -1674,7 +1676,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F6" s="13">
         <v>1219</v>
@@ -1691,7 +1693,7 @@
         <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>47</v>
@@ -1700,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F7" s="13">
         <v>1219</v>
@@ -1717,7 +1719,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>47</v>
@@ -1726,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F8" s="13">
         <v>1219</v>
@@ -1746,7 +1748,7 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>47</v>
@@ -1755,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F9" s="13">
         <v>1219</v>
@@ -1775,7 +1777,7 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>47</v>
@@ -1784,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F10" s="13">
         <v>1219</v>
@@ -1804,7 +1806,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>47</v>
@@ -1813,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F11" s="13">
         <v>1219</v>
@@ -1839,10 +1841,10 @@
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>47</v>
@@ -1851,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>52</v>
@@ -1871,10 +1873,10 @@
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>47</v>
@@ -1883,7 +1885,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>52</v>
@@ -1897,10 +1899,10 @@
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>47</v>
@@ -1909,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>52</v>
@@ -1923,10 +1925,10 @@
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>47</v>
@@ -1935,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>52</v>
@@ -1949,10 +1951,10 @@
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>47</v>
@@ -1961,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>52</v>
@@ -1975,10 +1977,10 @@
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>47</v>
@@ -1987,7 +1989,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>52</v>
@@ -2001,10 +2003,10 @@
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>47</v>
@@ -2013,7 +2015,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>52</v>
@@ -2042,7 +2044,7 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>47</v>
@@ -2051,7 +2053,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F21" s="13">
         <v>427</v>
@@ -2074,7 +2076,7 @@
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>47</v>
@@ -2083,7 +2085,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F22" s="13">
         <v>427</v>
@@ -2103,7 +2105,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>47</v>
@@ -2112,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F23" s="13">
         <v>427</v>
@@ -2138,7 +2140,7 @@
         <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>47</v>
@@ -2147,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F25" s="13">
         <v>21497</v>
@@ -2170,7 +2172,7 @@
         <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>47</v>
@@ -2179,7 +2181,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F26" s="13">
         <v>21497</v>
@@ -2196,7 +2198,7 @@
         <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>47</v>
@@ -2205,7 +2207,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F27" s="13">
         <v>21497</v>
@@ -2222,7 +2224,7 @@
         <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>47</v>
@@ -2231,7 +2233,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F28" s="13">
         <v>21497</v>
@@ -2248,7 +2250,7 @@
         <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>47</v>
@@ -2257,7 +2259,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F29" s="13">
         <v>21497</v>
@@ -2274,7 +2276,7 @@
         <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>47</v>
@@ -2283,7 +2285,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F30" s="13">
         <v>21497</v>
@@ -2300,7 +2302,7 @@
         <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>47</v>
@@ -2309,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F31" s="13">
         <v>21497</v>
@@ -2326,7 +2328,7 @@
         <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>47</v>
@@ -2335,7 +2337,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F32" s="13">
         <v>21497</v>
@@ -2352,7 +2354,7 @@
         <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>47</v>
@@ -2361,7 +2363,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F33" s="13">
         <v>21497</v>
@@ -2383,11 +2385,11 @@
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>58</v>
+      <c r="A35" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>47</v>
@@ -2396,10 +2398,10 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>5</v>
@@ -2415,11 +2417,11 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>58</v>
+      <c r="A36" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>47</v>
@@ -2428,10 +2430,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>6</v>
@@ -2441,11 +2443,11 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>58</v>
+      <c r="A37" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>47</v>
@@ -2454,10 +2456,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>7</v>
@@ -2467,11 +2469,11 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>58</v>
+      <c r="A38" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>47</v>
@@ -2480,10 +2482,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>29</v>
@@ -2503,11 +2505,11 @@
       <c r="H39" s="26"/>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>59</v>
+      <c r="A40" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>47</v>
@@ -2516,10 +2518,10 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>5</v>
@@ -2535,11 +2537,11 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>59</v>
+      <c r="A41" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>47</v>
@@ -2548,10 +2550,10 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>6</v>
@@ -2561,11 +2563,11 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>59</v>
+      <c r="A42" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>47</v>
@@ -2574,10 +2576,10 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>7</v>
@@ -2587,11 +2589,11 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>59</v>
+      <c r="A43" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>47</v>
@@ -2600,10 +2602,10 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>29</v>
@@ -2623,11 +2625,11 @@
       <c r="H44" s="26"/>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>60</v>
+      <c r="A45" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>47</v>
@@ -2636,10 +2638,10 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G45" s="13" t="s">
         <v>5</v>
@@ -2655,11 +2657,11 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>60</v>
+      <c r="A46" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>47</v>
@@ -2668,10 +2670,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>6</v>
@@ -2681,11 +2683,11 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>60</v>
+      <c r="A47" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>47</v>
@@ -2694,10 +2696,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>7</v>
@@ -2707,11 +2709,11 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>60</v>
+      <c r="A48" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>47</v>
@@ -2720,10 +2722,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>29</v>
@@ -2743,11 +2745,11 @@
       <c r="H49" s="26"/>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>61</v>
+      <c r="A50" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>47</v>
@@ -2756,10 +2758,10 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>5</v>
@@ -2775,11 +2777,11 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
-        <v>61</v>
+      <c r="A51" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>47</v>
@@ -2788,10 +2790,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>6</v>
@@ -2801,11 +2803,11 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
-        <v>61</v>
+      <c r="A52" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>47</v>
@@ -2814,10 +2816,10 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G52" s="13" t="s">
         <v>7</v>
@@ -2827,11 +2829,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>61</v>
+      <c r="A53" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>47</v>
@@ -2840,10 +2842,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G53" s="13" t="s">
         <v>29</v>
@@ -2863,11 +2865,11 @@
       <c r="H54" s="26"/>
     </row>
     <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
-        <v>62</v>
+      <c r="A55" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>47</v>
@@ -2876,10 +2878,10 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>5</v>
@@ -2895,11 +2897,11 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
-        <v>62</v>
+      <c r="A56" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>47</v>
@@ -2908,10 +2910,10 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>6</v>
@@ -2921,11 +2923,11 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>62</v>
+      <c r="A57" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>47</v>
@@ -2934,10 +2936,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G57" s="13" t="s">
         <v>7</v>
@@ -2947,11 +2949,11 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
-        <v>62</v>
+      <c r="A58" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>47</v>
@@ -2960,10 +2962,10 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>29</v>
@@ -2983,11 +2985,11 @@
       <c r="H59" s="26"/>
     </row>
     <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
-        <v>63</v>
+      <c r="A60" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>47</v>
@@ -2996,10 +2998,10 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F60" s="26" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>5</v>
@@ -3015,11 +3017,11 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>63</v>
+      <c r="A61" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>47</v>
@@ -3028,10 +3030,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F61" s="26" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>6</v>
@@ -3041,11 +3043,11 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
-        <v>63</v>
+      <c r="A62" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>47</v>
@@ -3054,10 +3056,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F62" s="26" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>7</v>
@@ -3067,11 +3069,11 @@
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
-        <v>63</v>
+      <c r="A63" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>47</v>
@@ -3080,10 +3082,10 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F63" s="26" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>29</v>
@@ -3102,24 +3104,24 @@
       <c r="G64" s="13"/>
       <c r="H64" s="26"/>
     </row>
-    <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
-        <v>64</v>
+    <row r="65" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="B65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D65" s="13">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D65" s="13">
-        <v>1</v>
-      </c>
-      <c r="E65" t="s">
-        <v>97</v>
-      </c>
       <c r="F65" s="24" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>5</v>
@@ -3134,24 +3136,24 @@
         <v>250</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
-        <v>64</v>
+    <row r="66" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="B66" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D66" s="13">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
         <v>86</v>
       </c>
-      <c r="C66" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D66" s="13">
-        <v>1</v>
-      </c>
-      <c r="E66" t="s">
-        <v>97</v>
-      </c>
       <c r="F66" s="24" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>6</v>
@@ -3160,24 +3162,24 @@
         <v>-42.495666666666665</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
-        <v>64</v>
+    <row r="67" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="B67" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D67" s="13">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D67" s="13">
-        <v>1</v>
-      </c>
-      <c r="E67" t="s">
-        <v>97</v>
-      </c>
       <c r="F67" s="24" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>7</v>
@@ -3186,24 +3188,24 @@
         <v>-42.122</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
-        <v>64</v>
+    <row r="68" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="B68" t="s">
+        <v>75</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" s="13">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
         <v>86</v>
       </c>
-      <c r="C68" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" s="13">
-        <v>1</v>
-      </c>
-      <c r="E68" t="s">
-        <v>97</v>
-      </c>
       <c r="F68" s="24" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>29</v>
@@ -3212,7 +3214,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69"/>
       <c r="C69" s="14"/>
@@ -3222,12 +3224,12 @@
       <c r="G69" s="13"/>
       <c r="H69" s="26"/>
     </row>
-    <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
-        <v>65</v>
+    <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B70" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>47</v>
@@ -3236,10 +3238,10 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>5</v>
@@ -3254,12 +3256,12 @@
         <v>350</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
-        <v>65</v>
+    <row r="71" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>47</v>
@@ -3268,10 +3270,10 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>6</v>
@@ -3280,12 +3282,12 @@
         <v>-42.495666666666665</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
-        <v>65</v>
+    <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B72" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>47</v>
@@ -3294,10 +3296,10 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>7</v>
@@ -3306,12 +3308,12 @@
         <v>-42.122</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
-        <v>65</v>
+    <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B73" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>47</v>
@@ -3320,10 +3322,10 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>29</v>
@@ -3332,7 +3334,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74"/>
       <c r="C74" s="14"/>
@@ -3342,12 +3344,12 @@
       <c r="G74" s="13"/>
       <c r="H74" s="26"/>
     </row>
-    <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="s">
-        <v>66</v>
+    <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="B75" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>47</v>
@@ -3356,10 +3358,10 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F75" s="24" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>5</v>
@@ -3374,12 +3376,12 @@
         <v>501</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="s">
-        <v>66</v>
+    <row r="76" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="B76" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>47</v>
@@ -3388,10 +3390,10 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>6</v>
@@ -3400,12 +3402,12 @@
         <v>-42.495666666666665</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="13" t="s">
-        <v>66</v>
+    <row r="77" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>47</v>
@@ -3414,10 +3416,10 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>7</v>
@@ -3426,12 +3428,12 @@
         <v>-42.122</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="s">
-        <v>66</v>
+    <row r="78" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>47</v>
@@ -3440,10 +3442,10 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>29</v>
@@ -3452,7 +3454,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79"/>
       <c r="C79" s="14"/>
@@ -3462,12 +3464,12 @@
       <c r="G79" s="13"/>
       <c r="H79" s="26"/>
     </row>
-    <row r="80" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="s">
-        <v>67</v>
+    <row r="80" spans="1:12" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B80" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>47</v>
@@ -3476,10 +3478,10 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F80" s="25" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G80" s="16" t="s">
         <v>5</v>
@@ -3493,13 +3495,14 @@
       <c r="J80" s="1">
         <v>748</v>
       </c>
+      <c r="L80" s="2"/>
     </row>
     <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="13" t="s">
-        <v>67</v>
+      <c r="A81" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B81" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>47</v>
@@ -3508,10 +3511,10 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>6</v>
@@ -3521,11 +3524,11 @@
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="13" t="s">
-        <v>67</v>
+      <c r="A82" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B82" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C82" s="14" t="s">
         <v>47</v>
@@ -3534,10 +3537,10 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>7</v>
@@ -3547,11 +3550,11 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="13" t="s">
-        <v>67</v>
+      <c r="A83" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B83" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C83" s="14" t="s">
         <v>47</v>
@@ -3560,10 +3563,10 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>29</v>
@@ -3583,11 +3586,11 @@
       <c r="H84" s="26"/>
     </row>
     <row r="85" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="s">
-        <v>68</v>
+      <c r="A85" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B85" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>47</v>
@@ -3596,10 +3599,10 @@
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>5</v>
@@ -3615,11 +3618,11 @@
       </c>
     </row>
     <row r="86" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="s">
-        <v>68</v>
+      <c r="A86" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>47</v>
@@ -3628,10 +3631,10 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>6</v>
@@ -3641,11 +3644,11 @@
       </c>
     </row>
     <row r="87" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
-        <v>68</v>
+      <c r="A87" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B87" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>47</v>
@@ -3654,10 +3657,10 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F87" s="24" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>7</v>
@@ -3667,11 +3670,11 @@
       </c>
     </row>
     <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="13" t="s">
-        <v>68</v>
+      <c r="A88" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B88" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>47</v>
@@ -3680,10 +3683,10 @@
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F88" s="24" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>29</v>
@@ -3703,11 +3706,11 @@
       <c r="H89" s="26"/>
     </row>
     <row r="90" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="13" t="s">
-        <v>69</v>
+      <c r="A90" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B90" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>47</v>
@@ -3716,10 +3719,10 @@
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F90" s="24" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>5</v>
@@ -3735,11 +3738,11 @@
       </c>
     </row>
     <row r="91" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="13" t="s">
-        <v>69</v>
+      <c r="A91" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B91" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>47</v>
@@ -3748,10 +3751,10 @@
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F91" s="24" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>6</v>
@@ -3761,11 +3764,11 @@
       </c>
     </row>
     <row r="92" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="13" t="s">
-        <v>69</v>
+      <c r="A92" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B92" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C92" s="14" t="s">
         <v>47</v>
@@ -3774,10 +3777,10 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F92" s="24" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>7</v>
@@ -3787,11 +3790,11 @@
       </c>
     </row>
     <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="13" t="s">
-        <v>69</v>
+      <c r="A93" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B93" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>47</v>
@@ -3800,10 +3803,10 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F93" s="24" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>29</v>
@@ -3824,10 +3827,10 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C95" s="13" t="s">
         <v>47</v>
@@ -3836,7 +3839,7 @@
         <v>1</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="F95" s="13">
         <v>13993</v>
@@ -3849,10 +3852,10 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C96" s="13" t="s">
         <v>47</v>
@@ -3861,7 +3864,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="F96" s="13">
         <v>13998</v>

</xml_diff>

<commit_message>
Argentine Basin - fixed deployment dates
Fixed deployment dates based on cruise reports and WHOI documentation
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA03FLMB_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA03FLMB_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7180" yWindow="8680" windowWidth="25960" windowHeight="10060" activeTab="1"/>
+    <workbookView xWindow="7180" yWindow="8680" windowWidth="25960" windowHeight="10060"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -1070,14 +1070,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Read Me"/>
       <sheetName val="Moorings"/>
-      <sheetName val="Asset_Cal_Info"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1372,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1453,7 +1449,7 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="G2" s="7">
-        <v>42328</v>
+        <v>42326</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>50</v>
@@ -1498,7 +1494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>

</xml_diff>